<commit_message>
test layout xlsx color coded complete
</commit_message>
<xml_diff>
--- a/Test_layout-color_coded.xlsx
+++ b/Test_layout-color_coded.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="19480"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="19480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,12 +103,6 @@
     <t>White: Door Direction Tests</t>
   </si>
   <si>
-    <t>Light Purple: walkway test scenarios</t>
-  </si>
-  <si>
-    <t>Light Blue: test targets</t>
-  </si>
-  <si>
     <t>Number of Doors: 15</t>
   </si>
   <si>
@@ -119,6 +113,12 @@
   </si>
   <si>
     <t>Yellow: adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Light Red: walkway test scenarios</t>
+  </si>
+  <si>
+    <t>Light Green: test targets</t>
   </si>
 </sst>
 </file>
@@ -140,7 +140,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,8 +189,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -198,11 +210,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF92D050"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF92D050"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF92D050"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF92D050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,16 +244,19 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,7 +265,25 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -545,7 +593,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -564,13 +612,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -582,7 +630,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -606,10 +654,10 @@
       <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="9" t="s">
+      <c r="R1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T1" s="5" t="s">
@@ -647,7 +695,7 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -665,7 +713,7 @@
       <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -689,7 +737,7 @@
       <c r="R2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
@@ -727,7 +775,7 @@
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -742,7 +790,7 @@
       <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -801,7 +849,7 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -929,13 +977,13 @@
       <c r="R5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="U5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="V5" s="3" t="s">
@@ -947,7 +995,7 @@
       <c r="X5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Y5" s="17" t="s">
         <v>1</v>
       </c>
       <c r="Z5" s="1">
@@ -1024,10 +1072,10 @@
       <c r="W6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="3" t="s">
+      <c r="X6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Z6" s="1">
@@ -1035,25 +1083,25 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="D7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1107,7 +1155,7 @@
       <c r="X7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Y7" s="5" t="s">
+      <c r="Y7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="Z7" s="1">
@@ -1121,16 +1169,16 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1261,7 +1309,7 @@
       <c r="V9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="W9" s="7" t="s">
+      <c r="W9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="X9" s="2" t="s">
@@ -1338,13 +1386,13 @@
       <c r="U10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="X10" s="3" t="s">
+      <c r="V10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="X10" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Y10" s="3" t="s">
@@ -1355,7 +1403,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1418,13 +1466,13 @@
       <c r="U11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="X11" s="3" t="s">
+      <c r="V11" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="W11" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" s="19" t="s">
         <v>1</v>
       </c>
       <c r="Y11" s="3" t="s">
@@ -1435,10 +1483,10 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1501,7 +1549,7 @@
       <c r="V12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W12" s="5" t="s">
+      <c r="W12" s="18" t="s">
         <v>16</v>
       </c>
       <c r="X12" s="5" t="s">
@@ -1515,7 +1563,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1616,7 +1664,7 @@
       <c r="G14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="13" t="s">
         <v>1</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -1693,13 +1741,13 @@
       <c r="F15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="G15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="13" t="s">
         <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
@@ -1708,7 +1756,7 @@
       <c r="K15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="M15" s="5" t="s">
@@ -1776,7 +1824,7 @@
       <c r="G16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="13" t="s">
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -1850,7 +1898,7 @@
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1883,7 +1931,7 @@
       <c r="P17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="12" t="s">
+      <c r="Q17" s="8" t="s">
         <v>1</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -1930,10 +1978,10 @@
       <c r="E18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
@@ -1942,7 +1990,7 @@
       <c r="I18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1963,10 +2011,10 @@
       <c r="P18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" s="12" t="s">
+      <c r="Q18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="8" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="3" t="s">
@@ -2010,13 +2058,13 @@
       <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="16" t="s">
         <v>1</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -2052,7 +2100,7 @@
       <c r="S19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T19" s="3" t="s">
+      <c r="T19" s="16" t="s">
         <v>1</v>
       </c>
       <c r="U19" s="3" t="s">
@@ -2093,13 +2141,13 @@
       <c r="F20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="16" t="s">
         <v>1</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="16" t="s">
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -2135,7 +2183,7 @@
       <c r="T20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="U20" s="13" t="s">
         <v>1</v>
       </c>
       <c r="V20" s="2" t="s">
@@ -2170,7 +2218,7 @@
       <c r="E21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -2212,10 +2260,10 @@
       <c r="S21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="U21" s="3" t="s">
+      <c r="T21" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U21" s="13" t="s">
         <v>1</v>
       </c>
       <c r="V21" s="2" t="s">
@@ -2227,7 +2275,7 @@
       <c r="X21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y21" s="7" t="s">
+      <c r="Y21" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Z21" s="1">
@@ -2312,116 +2360,116 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+    </row>
+    <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-    </row>
-    <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+    </row>
+    <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-    </row>
-    <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
all of our tests besides calc6steps working
</commit_message>
<xml_diff>
--- a/Test_layout-color_coded.xlsx
+++ b/Test_layout-color_coded.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hayden/Documents/Java/ClueGameExp/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15045" windowHeight="4905"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="19480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="30">
   <si>
     <t>X</t>
   </si>
@@ -96,18 +100,12 @@
     <t>DL</t>
   </si>
   <si>
-    <t>White: Door Direction Tests</t>
-  </si>
-  <si>
     <t>Number of Doors: 15</t>
   </si>
   <si>
     <t>Green: Adjacency list tests, inside room</t>
   </si>
   <si>
-    <t>Purple: Adjacency list tests, room door exits</t>
-  </si>
-  <si>
     <t>Yellow: adjacency lists beside room entrance</t>
   </si>
   <si>
@@ -115,6 +113,9 @@
   </si>
   <si>
     <t>Light Green: test targets</t>
+  </si>
+  <si>
+    <t>Purple: Adjacency list tests/Door Direction Tests</t>
   </si>
 </sst>
 </file>
@@ -589,16 +590,16 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="3.7109375" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="3.28515625" style="1"/>
+    <col min="1" max="26" width="3.6640625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="3.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -678,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -758,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -838,7 +839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -918,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -998,7 +999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1078,7 +1079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1718,7 +1719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1958,7 +1959,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2198,7 +2199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -2355,9 +2356,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2371,10 +2372,8 @@
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
     </row>
-    <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>24</v>
-      </c>
+    <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -2387,9 +2386,9 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
     </row>
-    <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2403,9 +2402,9 @@
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
     </row>
-    <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -2419,9 +2418,9 @@
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
     </row>
-    <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -2435,9 +2434,9 @@
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
     </row>
-    <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -2451,9 +2450,9 @@
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
     </row>
-    <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -2488,7 +2487,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2500,7 +2499,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>